<commit_message>
Extrema Pobreza retirado, estava limitando a tabela
</commit_message>
<xml_diff>
--- a/Projeto3/Dados.xlsx
+++ b/Projeto3/Dados.xlsx
@@ -17,14 +17,14 @@
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$G$209</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$F$209</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="271">
   <si>
     <t>Total expenditure on health as percentage of GDP (gross domestic product)</t>
   </si>
@@ -825,9 +825,6 @@
   </si>
   <si>
     <t>School</t>
-  </si>
-  <si>
-    <t>Poverty</t>
   </si>
   <si>
     <t>Child</t>
@@ -849,7 +846,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -880,13 +877,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -943,12 +935,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -967,7 +953,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1023,26 +1009,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1384,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G276"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1400,30 +1377,27 @@
     <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="F1" s="27" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>269</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>268</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>265</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>266</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>267</v>
-      </c>
-      <c r="G1" s="32" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>214</v>
       </c>
@@ -1431,10 +1405,9 @@
       <c r="C2" s="15"/>
       <c r="D2" s="19"/>
       <c r="E2" s="20"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="30"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F2" s="25"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
@@ -1448,10 +1421,9 @@
         <v>35</v>
       </c>
       <c r="E3" s="20"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="30"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F3" s="25"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>215</v>
       </c>
@@ -1459,10 +1431,9 @@
       <c r="C4" s="15"/>
       <c r="D4" s="19"/>
       <c r="E4" s="20"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="30"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F4" s="25"/>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>2</v>
       </c>
@@ -1476,12 +1447,11 @@
         <v>91</v>
       </c>
       <c r="E5" s="20"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="31">
+      <c r="F5" s="26">
         <v>2879.57</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>3</v>
       </c>
@@ -1497,14 +1467,11 @@
       <c r="E6" s="20">
         <v>96.395089999999996</v>
       </c>
-      <c r="F6" s="24">
-        <v>3.01</v>
-      </c>
-      <c r="G6" s="31">
+      <c r="F6" s="26">
         <v>3153.38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>4</v>
       </c>
@@ -1514,12 +1481,9 @@
       <c r="C7" s="15"/>
       <c r="D7" s="19"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="24">
-        <v>3.37</v>
-      </c>
-      <c r="G7" s="30"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F7" s="25"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>5</v>
       </c>
@@ -1533,10 +1497,9 @@
         <v>100</v>
       </c>
       <c r="E8" s="20"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="30"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F8" s="25"/>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>6</v>
       </c>
@@ -1550,12 +1513,11 @@
         <v>52</v>
       </c>
       <c r="E9" s="20"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="31">
+      <c r="F9" s="26">
         <v>1973.29</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>216</v>
       </c>
@@ -1563,10 +1525,9 @@
       <c r="C10" s="15"/>
       <c r="D10" s="19"/>
       <c r="E10" s="20"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="30"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>7</v>
       </c>
@@ -1578,12 +1539,11 @@
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="31">
+      <c r="F11" s="26">
         <v>2368.5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>8</v>
       </c>
@@ -1599,12 +1559,11 @@
       <c r="E12" s="20">
         <v>102.61247</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="31">
+      <c r="F12" s="26">
         <v>2940.98</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>9</v>
       </c>
@@ -1620,14 +1579,11 @@
       <c r="E13" s="20">
         <v>101.31553</v>
       </c>
-      <c r="F13" s="24">
-        <v>0</v>
-      </c>
-      <c r="G13" s="31">
+      <c r="F13" s="26">
         <v>2279.87</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>10</v>
       </c>
@@ -1641,10 +1597,9 @@
       <c r="E14" s="20">
         <v>93.320849999999993</v>
       </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="30"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F14" s="25"/>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>11</v>
       </c>
@@ -1658,12 +1613,11 @@
         <v>100</v>
       </c>
       <c r="E15" s="20"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="31">
+      <c r="F15" s="26">
         <v>3227.05</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>12</v>
       </c>
@@ -1679,12 +1633,11 @@
       <c r="E16" s="20">
         <v>103.44956000000001</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="31">
+      <c r="F16" s="26">
         <v>3818.8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>13</v>
       </c>
@@ -1700,14 +1653,11 @@
       <c r="E17" s="20">
         <v>98.130369999999999</v>
       </c>
-      <c r="F17" s="24">
-        <v>10.220000000000001</v>
-      </c>
-      <c r="G17" s="31">
+      <c r="F17" s="26">
         <v>2961.19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>14</v>
       </c>
@@ -1723,14 +1673,11 @@
       <c r="E18" s="20">
         <v>102.36646</v>
       </c>
-      <c r="F18" s="24">
-        <v>12.19</v>
-      </c>
-      <c r="G18" s="31">
+      <c r="F18" s="26">
         <v>2712.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>15</v>
       </c>
@@ -1742,12 +1689,9 @@
       </c>
       <c r="D19" s="19"/>
       <c r="E19" s="20"/>
-      <c r="F19" s="24">
-        <v>0.04</v>
-      </c>
-      <c r="G19" s="30"/>
-    </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F19" s="25"/>
+    </row>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>16</v>
       </c>
@@ -1761,12 +1705,11 @@
         <v>52</v>
       </c>
       <c r="E20" s="20"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="31">
+      <c r="F20" s="26">
         <v>2281.1799999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>17</v>
       </c>
@@ -1782,14 +1725,11 @@
       <c r="E21" s="20">
         <v>91.587339999999998</v>
       </c>
-      <c r="F21" s="24">
-        <v>5.84</v>
-      </c>
-      <c r="G21" s="31">
+      <c r="F21" s="26">
         <v>3055.81</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>18</v>
       </c>
@@ -1805,14 +1745,11 @@
       <c r="E22" s="20">
         <v>92.856409999999997</v>
       </c>
-      <c r="F22" s="24">
-        <v>0.26</v>
-      </c>
-      <c r="G22" s="31">
+      <c r="F22" s="26">
         <v>3145.64</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>19</v>
       </c>
@@ -1828,12 +1765,11 @@
       <c r="E23" s="20">
         <v>89.616100000000003</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="31">
+      <c r="F23" s="26">
         <v>3693.57</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>20</v>
       </c>
@@ -1849,12 +1785,11 @@
       <c r="E24" s="20">
         <v>99.061989999999994</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="31">
+      <c r="F24" s="26">
         <v>2717.57</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>21</v>
       </c>
@@ -1868,14 +1803,11 @@
         <v>12</v>
       </c>
       <c r="E25" s="20"/>
-      <c r="F25" s="24">
-        <v>30.82</v>
-      </c>
-      <c r="G25" s="31">
+      <c r="F25" s="26">
         <v>2532.92</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>22</v>
       </c>
@@ -1885,14 +1817,11 @@
       <c r="C26" s="15"/>
       <c r="D26" s="19"/>
       <c r="E26" s="20"/>
-      <c r="F26" s="24">
-        <v>27.61</v>
-      </c>
-      <c r="G26" s="31">
+      <c r="F26" s="26">
         <v>2597.9899999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>23</v>
       </c>
@@ -1906,12 +1835,9 @@
         <v>42</v>
       </c>
       <c r="E27" s="20"/>
-      <c r="F27" s="24">
-        <v>0.34</v>
-      </c>
-      <c r="G27" s="30"/>
-    </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F27" s="25"/>
+    </row>
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>24</v>
       </c>
@@ -1927,12 +1853,11 @@
       <c r="E28" s="20">
         <v>98.488950000000003</v>
       </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="31">
+      <c r="F28" s="26">
         <v>2064.13</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>25</v>
       </c>
@@ -1946,12 +1871,11 @@
         <v>95</v>
       </c>
       <c r="E29" s="20"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="31">
+      <c r="F29" s="26">
         <v>3078.06</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>26</v>
       </c>
@@ -1967,12 +1891,11 @@
       <c r="E30" s="20">
         <v>94.160470000000004</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="31">
+      <c r="F30" s="26">
         <v>2263.8200000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>27</v>
       </c>
@@ -1986,12 +1909,11 @@
         <v>78</v>
       </c>
       <c r="E31" s="20"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="31">
+      <c r="F31" s="26">
         <v>3112.51</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>217</v>
       </c>
@@ -1999,10 +1921,9 @@
       <c r="C32" s="15"/>
       <c r="D32" s="19"/>
       <c r="E32" s="20"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="30"/>
-    </row>
-    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F32" s="25"/>
+    </row>
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
         <v>28</v>
       </c>
@@ -2016,14 +1937,11 @@
       <c r="E33" s="20">
         <v>117.24621999999999</v>
       </c>
-      <c r="F33" s="24">
-        <v>8.84</v>
-      </c>
-      <c r="G33" s="31">
+      <c r="F33" s="26">
         <v>2968.12</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>29</v>
       </c>
@@ -2039,12 +1957,11 @@
       <c r="E34" s="20">
         <v>98.287350000000004</v>
       </c>
-      <c r="F34" s="23"/>
-      <c r="G34" s="31">
+      <c r="F34" s="26">
         <v>2766.11</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
         <v>30</v>
       </c>
@@ -2060,12 +1977,11 @@
       <c r="E35" s="20">
         <v>33.107469999999999</v>
       </c>
-      <c r="F35" s="23"/>
-      <c r="G35" s="31">
+      <c r="F35" s="26">
         <v>2676.91</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>31</v>
       </c>
@@ -2081,12 +1997,11 @@
       <c r="E36" s="20">
         <v>41.90269</v>
       </c>
-      <c r="F36" s="23"/>
-      <c r="G36" s="31">
+      <c r="F36" s="26">
         <v>1684.72</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>32</v>
       </c>
@@ -2102,14 +2017,11 @@
       <c r="E37" s="20">
         <v>90.967889999999997</v>
       </c>
-      <c r="F37" s="24">
-        <v>2.06</v>
-      </c>
-      <c r="G37" s="31">
+      <c r="F37" s="26">
         <v>2267.5500000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>33</v>
       </c>
@@ -2125,12 +2037,11 @@
       <c r="E38" s="20">
         <v>57.114530000000002</v>
       </c>
-      <c r="F38" s="23"/>
-      <c r="G38" s="31">
+      <c r="F38" s="26">
         <v>2269.12</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>34</v>
       </c>
@@ -2144,12 +2055,11 @@
         <v>100</v>
       </c>
       <c r="E39" s="20"/>
-      <c r="F39" s="23"/>
-      <c r="G39" s="31">
+      <c r="F39" s="26">
         <v>3532.47</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>35</v>
       </c>
@@ -2165,12 +2075,11 @@
       <c r="E40" s="20">
         <v>93.055319999999995</v>
       </c>
-      <c r="F40" s="23"/>
-      <c r="G40" s="31">
+      <c r="F40" s="26">
         <v>2571.92</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>218</v>
       </c>
@@ -2180,12 +2089,9 @@
         <v>96</v>
       </c>
       <c r="E41" s="20"/>
-      <c r="F41" s="24">
-        <v>0.39</v>
-      </c>
-      <c r="G41" s="30"/>
-    </row>
-    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F41" s="25"/>
+    </row>
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>36</v>
       </c>
@@ -2201,12 +2107,11 @@
       <c r="E42" s="20">
         <v>33.183450000000001</v>
       </c>
-      <c r="F42" s="23"/>
-      <c r="G42" s="31">
+      <c r="F42" s="26">
         <v>1985.84</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>37</v>
       </c>
@@ -2220,14 +2125,11 @@
         <v>12</v>
       </c>
       <c r="E43" s="20"/>
-      <c r="F43" s="24">
-        <v>3.72</v>
-      </c>
-      <c r="G43" s="31">
+      <c r="F43" s="26">
         <v>2055.8200000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>38</v>
       </c>
@@ -2239,12 +2141,9 @@
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="20"/>
-      <c r="F44" s="24">
-        <v>6.94</v>
-      </c>
-      <c r="G44" s="30"/>
-    </row>
-    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F44" s="25"/>
+    </row>
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>39</v>
       </c>
@@ -2260,12 +2159,11 @@
       <c r="E45" s="20">
         <v>95.720770000000002</v>
       </c>
-      <c r="F45" s="23"/>
-      <c r="G45" s="31">
+      <c r="F45" s="26">
         <v>2920.42</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>40</v>
       </c>
@@ -2279,14 +2177,11 @@
         <v>57</v>
       </c>
       <c r="E46" s="20"/>
-      <c r="F46" s="24">
-        <v>2.85</v>
-      </c>
-      <c r="G46" s="31">
+      <c r="F46" s="26">
         <v>2980.54</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>219</v>
       </c>
@@ -2294,10 +2189,9 @@
       <c r="C47" s="15"/>
       <c r="D47" s="19"/>
       <c r="E47" s="20"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="30"/>
-    </row>
-    <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F47" s="25"/>
+    </row>
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
         <v>220</v>
       </c>
@@ -2305,10 +2199,9 @@
       <c r="C48" s="15"/>
       <c r="D48" s="19"/>
       <c r="E48" s="20"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="30"/>
-    </row>
-    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F48" s="25"/>
+    </row>
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
         <v>41</v>
       </c>
@@ -2324,14 +2217,11 @@
       <c r="E49" s="20">
         <v>111.27198</v>
       </c>
-      <c r="F49" s="24">
-        <v>0.47</v>
-      </c>
-      <c r="G49" s="31">
+      <c r="F49" s="26">
         <v>2684.65</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
         <v>42</v>
       </c>
@@ -2347,12 +2237,11 @@
       <c r="E50" s="20">
         <v>67.022400000000005</v>
       </c>
-      <c r="F50" s="23"/>
-      <c r="G50" s="31">
+      <c r="F50" s="26">
         <v>1884.49</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
         <v>43</v>
       </c>
@@ -2368,12 +2257,11 @@
       <c r="E51" s="20">
         <v>50.473199999999999</v>
       </c>
-      <c r="F51" s="23"/>
-      <c r="G51" s="31">
+      <c r="F51" s="26">
         <v>1605.08</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>44</v>
       </c>
@@ -2389,14 +2277,11 @@
       <c r="E52" s="20">
         <v>76.111999999999995</v>
       </c>
-      <c r="F52" s="24">
-        <v>0</v>
-      </c>
-      <c r="G52" s="31">
+      <c r="F52" s="26">
         <v>2511.88</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>221</v>
       </c>
@@ -2406,10 +2291,9 @@
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="20"/>
-      <c r="F53" s="23"/>
-      <c r="G53" s="30"/>
-    </row>
-    <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F53" s="25"/>
+    </row>
+    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
         <v>45</v>
       </c>
@@ -2425,12 +2309,11 @@
       <c r="E54" s="20">
         <v>92.386669999999995</v>
       </c>
-      <c r="F54" s="23"/>
-      <c r="G54" s="31">
+      <c r="F54" s="26">
         <v>2839.76</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
         <v>46</v>
       </c>
@@ -2446,12 +2329,11 @@
       <c r="E55" s="20">
         <v>47.570259999999998</v>
       </c>
-      <c r="F55" s="23"/>
-      <c r="G55" s="31">
+      <c r="F55" s="26">
         <v>2527.52</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>47</v>
       </c>
@@ -2467,14 +2349,11 @@
       <c r="E56" s="20">
         <v>101.07478999999999</v>
       </c>
-      <c r="F56" s="24">
-        <v>14.75</v>
-      </c>
-      <c r="G56" s="31">
+      <c r="F56" s="26">
         <v>2989.91</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>48</v>
       </c>
@@ -2490,14 +2369,11 @@
       <c r="E57" s="20">
         <v>91.732680000000002</v>
       </c>
-      <c r="F57" s="24">
-        <v>0</v>
-      </c>
-      <c r="G57" s="31">
+      <c r="F57" s="26">
         <v>3273.96</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>49</v>
       </c>
@@ -2513,12 +2389,11 @@
       <c r="E58" s="20">
         <v>99.951629999999994</v>
       </c>
-      <c r="F58" s="23"/>
-      <c r="G58" s="31">
+      <c r="F58" s="26">
         <v>3180.69</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
         <v>50</v>
       </c>
@@ -2534,14 +2409,11 @@
       <c r="E59" s="20">
         <v>93.148570000000007</v>
       </c>
-      <c r="F59" s="24">
-        <v>1.03</v>
-      </c>
-      <c r="G59" s="31">
+      <c r="F59" s="26">
         <v>3260.34</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>222</v>
       </c>
@@ -2549,10 +2421,9 @@
       <c r="C60" s="15"/>
       <c r="D60" s="19"/>
       <c r="E60" s="20"/>
-      <c r="F60" s="23"/>
-      <c r="G60" s="30"/>
-    </row>
-    <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F60" s="25"/>
+    </row>
+    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
         <v>51</v>
       </c>
@@ -2568,14 +2439,11 @@
       <c r="E61" s="20">
         <v>101.46519000000001</v>
       </c>
-      <c r="F61" s="24">
-        <v>39.33</v>
-      </c>
-      <c r="G61" s="31">
+      <c r="F61" s="26">
         <v>3415.88</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
         <v>52</v>
       </c>
@@ -2589,12 +2457,11 @@
         <v>52</v>
       </c>
       <c r="E62" s="20"/>
-      <c r="F62" s="23"/>
-      <c r="G62" s="31">
+      <c r="F62" s="26">
         <v>2291.39</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>53</v>
       </c>
@@ -2610,12 +2477,11 @@
       <c r="E63" s="20">
         <v>94.710509999999999</v>
       </c>
-      <c r="F63" s="23"/>
-      <c r="G63" s="31">
+      <c r="F63" s="26">
         <v>3157.16</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
         <v>54</v>
       </c>
@@ -2631,12 +2497,11 @@
       <c r="E64" s="20">
         <v>91.286510000000007</v>
       </c>
-      <c r="F64" s="23"/>
-      <c r="G64" s="31">
+      <c r="F64" s="26">
         <v>2295.1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
         <v>223</v>
       </c>
@@ -2644,12 +2509,9 @@
       <c r="C65" s="15"/>
       <c r="D65" s="19"/>
       <c r="E65" s="20"/>
-      <c r="F65" s="24">
-        <v>15.8</v>
-      </c>
-      <c r="G65" s="30"/>
-    </row>
-    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F65" s="25"/>
+    </row>
+    <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
         <v>55</v>
       </c>
@@ -2665,12 +2527,11 @@
       <c r="E66" s="20">
         <v>105.50139</v>
       </c>
-      <c r="F66" s="23"/>
-      <c r="G66" s="31">
+      <c r="F66" s="26">
         <v>2300.87</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
         <v>56</v>
       </c>
@@ -2686,12 +2547,11 @@
       <c r="E67" s="20">
         <v>95.774829999999994</v>
       </c>
-      <c r="F67" s="23"/>
-      <c r="G67" s="31">
+      <c r="F67" s="26">
         <v>3194.55</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
         <v>57</v>
       </c>
@@ -2707,12 +2567,11 @@
       <c r="E68" s="20">
         <v>88.735010000000003</v>
       </c>
-      <c r="F68" s="23"/>
-      <c r="G68" s="31">
+      <c r="F68" s="26">
         <v>2589.61</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
         <v>58</v>
       </c>
@@ -2726,10 +2585,9 @@
         <v>89</v>
       </c>
       <c r="E69" s="20"/>
-      <c r="F69" s="23"/>
-      <c r="G69" s="30"/>
-    </row>
-    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F69" s="25"/>
+    </row>
+    <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
         <v>59</v>
       </c>
@@ -2745,12 +2603,11 @@
       <c r="E70" s="20">
         <v>46.967269999999999</v>
       </c>
-      <c r="F70" s="23"/>
-      <c r="G70" s="31">
+      <c r="F70" s="26">
         <v>1605.4</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
         <v>224</v>
       </c>
@@ -2758,12 +2615,9 @@
       <c r="C71" s="15"/>
       <c r="D71" s="19"/>
       <c r="E71" s="20"/>
-      <c r="F71" s="24">
-        <v>3.37</v>
-      </c>
-      <c r="G71" s="30"/>
-    </row>
-    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F71" s="25"/>
+    </row>
+    <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
         <v>60</v>
       </c>
@@ -2779,14 +2633,11 @@
       <c r="E72" s="20">
         <v>98.884680000000003</v>
       </c>
-      <c r="F72" s="24">
-        <v>0</v>
-      </c>
-      <c r="G72" s="31">
+      <c r="F72" s="26">
         <v>3154.03</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
         <v>61</v>
       </c>
@@ -2802,14 +2653,11 @@
       <c r="E73" s="20">
         <v>48.334809999999997</v>
       </c>
-      <c r="F73" s="24">
-        <v>0.33</v>
-      </c>
-      <c r="G73" s="31">
+      <c r="F73" s="26">
         <v>1979.68</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
         <v>225</v>
       </c>
@@ -2817,10 +2665,9 @@
       <c r="C74" s="15"/>
       <c r="D74" s="19"/>
       <c r="E74" s="20"/>
-      <c r="F74" s="23"/>
-      <c r="G74" s="30"/>
-    </row>
-    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F74" s="25"/>
+    </row>
+    <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="17" t="s">
         <v>226</v>
       </c>
@@ -2828,10 +2675,9 @@
       <c r="C75" s="15"/>
       <c r="D75" s="19"/>
       <c r="E75" s="20"/>
-      <c r="F75" s="23"/>
-      <c r="G75" s="30"/>
-    </row>
-    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F75" s="25"/>
+    </row>
+    <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="17" t="s">
         <v>62</v>
       </c>
@@ -2847,12 +2693,11 @@
       <c r="E76" s="20">
         <v>102.84966</v>
       </c>
-      <c r="F76" s="23"/>
-      <c r="G76" s="31">
+      <c r="F76" s="26">
         <v>3041.15</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="17" t="s">
         <v>63</v>
       </c>
@@ -2868,12 +2713,11 @@
       <c r="E77" s="20">
         <v>98.316839999999999</v>
       </c>
-      <c r="F77" s="23"/>
-      <c r="G77" s="31">
+      <c r="F77" s="26">
         <v>3220.91</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="17" t="s">
         <v>64</v>
       </c>
@@ -2887,14 +2731,11 @@
         <v>100</v>
       </c>
       <c r="E78" s="20"/>
-      <c r="F78" s="24">
-        <v>0.16</v>
-      </c>
-      <c r="G78" s="31">
+      <c r="F78" s="26">
         <v>3532.24</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="17" t="s">
         <v>65</v>
       </c>
@@ -2906,10 +2747,9 @@
       </c>
       <c r="D79" s="19"/>
       <c r="E79" s="20"/>
-      <c r="F79" s="23"/>
-      <c r="G79" s="30"/>
-    </row>
-    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F79" s="25"/>
+    </row>
+    <row r="80" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
         <v>66</v>
       </c>
@@ -2923,12 +2763,11 @@
         <v>98</v>
       </c>
       <c r="E80" s="20"/>
-      <c r="F80" s="23"/>
-      <c r="G80" s="31">
+      <c r="F80" s="26">
         <v>2942.21</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="17" t="s">
         <v>67</v>
       </c>
@@ -2942,12 +2781,11 @@
         <v>33</v>
       </c>
       <c r="E81" s="20"/>
-      <c r="F81" s="23"/>
-      <c r="G81" s="31">
+      <c r="F81" s="26">
         <v>2754.9</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
         <v>68</v>
       </c>
@@ -2963,14 +2801,11 @@
       <c r="E82" s="20">
         <v>72.432400000000001</v>
       </c>
-      <c r="F82" s="24">
-        <v>1.9</v>
-      </c>
-      <c r="G82" s="31">
+      <c r="F82" s="26">
         <v>2384.59</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>69</v>
       </c>
@@ -2986,14 +2821,11 @@
       <c r="E83" s="20">
         <v>94.164230000000003</v>
       </c>
-      <c r="F83" s="24">
-        <v>35.1</v>
-      </c>
-      <c r="G83" s="31">
+      <c r="F83" s="26">
         <v>2859.39</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="17" t="s">
         <v>70</v>
       </c>
@@ -3009,12 +2841,11 @@
       <c r="E84" s="20">
         <v>102.74424999999999</v>
       </c>
-      <c r="F84" s="23"/>
-      <c r="G84" s="31">
+      <c r="F84" s="26">
         <v>3546.96</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
         <v>71</v>
       </c>
@@ -3030,12 +2861,11 @@
       <c r="E85" s="20">
         <v>77.907629999999997</v>
       </c>
-      <c r="F85" s="23"/>
-      <c r="G85" s="31">
+      <c r="F85" s="26">
         <v>2907.02</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
         <v>227</v>
       </c>
@@ -3043,12 +2873,9 @@
       <c r="C86" s="15"/>
       <c r="D86" s="19"/>
       <c r="E86" s="20"/>
-      <c r="F86" s="24">
-        <v>83.76</v>
-      </c>
-      <c r="G86" s="30"/>
-    </row>
-    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F86" s="25"/>
+    </row>
+    <row r="87" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
         <v>72</v>
       </c>
@@ -3064,12 +2891,11 @@
       <c r="E87" s="20">
         <v>100.93903</v>
       </c>
-      <c r="F87" s="23"/>
-      <c r="G87" s="31">
+      <c r="F87" s="26">
         <v>3724.69</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="17" t="s">
         <v>73</v>
       </c>
@@ -3081,10 +2907,9 @@
         <v>100</v>
       </c>
       <c r="E88" s="20"/>
-      <c r="F88" s="23"/>
-      <c r="G88" s="30"/>
-    </row>
-    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F88" s="25"/>
+    </row>
+    <row r="89" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
         <v>74</v>
       </c>
@@ -3100,12 +2925,11 @@
       <c r="E89" s="20">
         <v>97.641069999999999</v>
       </c>
-      <c r="F89" s="23"/>
-      <c r="G89" s="31">
+      <c r="F89" s="26">
         <v>2454.1799999999998</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
         <v>75</v>
       </c>
@@ -3117,10 +2941,9 @@
       </c>
       <c r="D90" s="19"/>
       <c r="E90" s="20"/>
-      <c r="F90" s="23"/>
-      <c r="G90" s="30"/>
-    </row>
-    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F90" s="25"/>
+    </row>
+    <row r="91" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="17" t="s">
         <v>76</v>
       </c>
@@ -3134,10 +2957,9 @@
         <v>99</v>
       </c>
       <c r="E91" s="20"/>
-      <c r="F91" s="23"/>
-      <c r="G91" s="30"/>
-    </row>
-    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F91" s="25"/>
+    </row>
+    <row r="92" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
         <v>77</v>
       </c>
@@ -3153,14 +2975,11 @@
       <c r="E92" s="20">
         <v>77.350830000000002</v>
       </c>
-      <c r="F92" s="24">
-        <v>0</v>
-      </c>
-      <c r="G92" s="31">
+      <c r="F92" s="26">
         <v>2159.2600000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>228</v>
       </c>
@@ -3168,10 +2987,9 @@
       <c r="C93" s="15"/>
       <c r="D93" s="19"/>
       <c r="E93" s="20"/>
-      <c r="F93" s="23"/>
-      <c r="G93" s="30"/>
-    </row>
-    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F93" s="25"/>
+    </row>
+    <row r="94" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
         <v>78</v>
       </c>
@@ -3187,12 +3005,11 @@
       <c r="E94" s="20">
         <v>63.726939999999999</v>
       </c>
-      <c r="F94" s="23"/>
-      <c r="G94" s="31">
+      <c r="F94" s="26">
         <v>2568.0300000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
         <v>79</v>
       </c>
@@ -3206,12 +3023,11 @@
         <v>18</v>
       </c>
       <c r="E95" s="20"/>
-      <c r="F95" s="23"/>
-      <c r="G95" s="31">
+      <c r="F95" s="26">
         <v>2306</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="17" t="s">
         <v>80</v>
       </c>
@@ -3227,12 +3043,11 @@
       <c r="E96" s="20">
         <v>98.505319999999998</v>
       </c>
-      <c r="F96" s="23"/>
-      <c r="G96" s="31">
+      <c r="F96" s="26">
         <v>2758.51</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="17" t="s">
         <v>81</v>
       </c>
@@ -3246,12 +3061,11 @@
         <v>18</v>
       </c>
       <c r="E97" s="20"/>
-      <c r="F97" s="23"/>
-      <c r="G97" s="31">
+      <c r="F97" s="26">
         <v>1869.77</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
         <v>229</v>
       </c>
@@ -3259,12 +3073,9 @@
       <c r="C98" s="15"/>
       <c r="D98" s="19"/>
       <c r="E98" s="20"/>
-      <c r="F98" s="24">
-        <v>1.01</v>
-      </c>
-      <c r="G98" s="30"/>
-    </row>
-    <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F98" s="25"/>
+    </row>
+    <row r="99" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="17" t="s">
         <v>82</v>
       </c>
@@ -3278,12 +3089,11 @@
         <v>73</v>
       </c>
       <c r="E99" s="20"/>
-      <c r="F99" s="23"/>
-      <c r="G99" s="31">
+      <c r="F99" s="26">
         <v>2623.41</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="17" t="s">
         <v>83</v>
       </c>
@@ -3297,12 +3107,9 @@
       <c r="E100" s="20">
         <v>101.40062</v>
       </c>
-      <c r="F100" s="24">
-        <v>0.37</v>
-      </c>
-      <c r="G100" s="30"/>
-    </row>
-    <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F100" s="25"/>
+    </row>
+    <row r="101" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="17" t="s">
         <v>84</v>
       </c>
@@ -3318,14 +3125,11 @@
       <c r="E101" s="20">
         <v>95.74982</v>
       </c>
-      <c r="F101" s="24">
-        <v>2.57</v>
-      </c>
-      <c r="G101" s="31">
+      <c r="F101" s="26">
         <v>3465.18</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="17" t="s">
         <v>85</v>
       </c>
@@ -3341,12 +3145,11 @@
       <c r="E102" s="20">
         <v>96.92407</v>
       </c>
-      <c r="F102" s="23"/>
-      <c r="G102" s="31">
+      <c r="F102" s="26">
         <v>3361.9</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="17" t="s">
         <v>86</v>
       </c>
@@ -3362,12 +3165,11 @@
       <c r="E103" s="20">
         <v>94.353080000000006</v>
       </c>
-      <c r="F103" s="23"/>
-      <c r="G103" s="31">
+      <c r="F103" s="26">
         <v>2351.86</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="17" t="s">
         <v>87</v>
       </c>
@@ -3383,12 +3185,11 @@
       <c r="E104" s="20">
         <v>102.29208</v>
       </c>
-      <c r="F104" s="23"/>
-      <c r="G104" s="31">
+      <c r="F104" s="26">
         <v>2538.42</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="17" t="s">
         <v>88</v>
       </c>
@@ -3404,14 +3205,11 @@
       <c r="E105" s="20">
         <v>95.736810000000006</v>
       </c>
-      <c r="F105" s="24">
-        <v>0.37</v>
-      </c>
-      <c r="G105" s="31">
+      <c r="F105" s="26">
         <v>3043.61</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="17" t="s">
         <v>89</v>
       </c>
@@ -3427,10 +3225,9 @@
       <c r="E106" s="20">
         <v>65.198809999999995</v>
       </c>
-      <c r="F106" s="23"/>
-      <c r="G106" s="30"/>
-    </row>
-    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F106" s="25"/>
+    </row>
+    <row r="107" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="17" t="s">
         <v>90</v>
       </c>
@@ -3444,12 +3241,11 @@
         <v>99</v>
       </c>
       <c r="E107" s="20"/>
-      <c r="F107" s="23"/>
-      <c r="G107" s="31">
+      <c r="F107" s="26">
         <v>3612.26</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="17" t="s">
         <v>230</v>
       </c>
@@ -3457,10 +3253,9 @@
       <c r="C108" s="15"/>
       <c r="D108" s="19"/>
       <c r="E108" s="20"/>
-      <c r="F108" s="23"/>
-      <c r="G108" s="30"/>
-    </row>
-    <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F108" s="25"/>
+    </row>
+    <row r="109" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="17" t="s">
         <v>91</v>
       </c>
@@ -3476,12 +3271,11 @@
       <c r="E109" s="20">
         <v>103.54721000000001</v>
       </c>
-      <c r="F109" s="23"/>
-      <c r="G109" s="31">
+      <c r="F109" s="26">
         <v>3527.47</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="17" t="s">
         <v>92</v>
       </c>
@@ -3495,14 +3289,11 @@
       <c r="E110" s="20">
         <v>101.28131</v>
       </c>
-      <c r="F110" s="24">
-        <v>0.33</v>
-      </c>
-      <c r="G110" s="31">
+      <c r="F110" s="26">
         <v>3645.65</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="17" t="s">
         <v>93</v>
       </c>
@@ -3518,12 +3309,11 @@
       <c r="E111" s="20">
         <v>84.330340000000007</v>
       </c>
-      <c r="F111" s="23"/>
-      <c r="G111" s="31">
+      <c r="F111" s="26">
         <v>2851.57</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="17" t="s">
         <v>94</v>
       </c>
@@ -3537,14 +3327,11 @@
         <v>100</v>
       </c>
       <c r="E112" s="20"/>
-      <c r="F112" s="24">
-        <v>7.2</v>
-      </c>
-      <c r="G112" s="31">
+      <c r="F112" s="26">
         <v>2812.14</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="17" t="s">
         <v>231</v>
       </c>
@@ -3552,10 +3339,9 @@
       <c r="C113" s="15"/>
       <c r="D113" s="19"/>
       <c r="E113" s="20"/>
-      <c r="F113" s="23"/>
-      <c r="G113" s="30"/>
-    </row>
-    <row r="114" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F113" s="25"/>
+    </row>
+    <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="17" t="s">
         <v>95</v>
       </c>
@@ -3571,14 +3357,11 @@
       <c r="E114" s="20">
         <v>103.92838999999999</v>
       </c>
-      <c r="F114" s="24">
-        <v>7.46</v>
-      </c>
-      <c r="G114" s="31">
+      <c r="F114" s="26">
         <v>3015.43</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="17" t="s">
         <v>96</v>
       </c>
@@ -3594,14 +3377,11 @@
       <c r="E115" s="20">
         <v>101.40773</v>
       </c>
-      <c r="F115" s="24">
-        <v>6.31</v>
-      </c>
-      <c r="G115" s="31">
+      <c r="F115" s="26">
         <v>3490.13</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="17" t="s">
         <v>97</v>
       </c>
@@ -3615,12 +3395,11 @@
         <v>30</v>
       </c>
       <c r="E116" s="20"/>
-      <c r="F116" s="23"/>
-      <c r="G116" s="31">
+      <c r="F116" s="26">
         <v>2089.31</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A117" s="17" t="s">
         <v>98</v>
       </c>
@@ -3636,14 +3415,11 @@
       <c r="E117" s="20">
         <v>121.83369</v>
       </c>
-      <c r="F117" s="24">
-        <v>0.02</v>
-      </c>
-      <c r="G117" s="31">
+      <c r="F117" s="26">
         <v>2899.07</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" s="17" t="s">
         <v>99</v>
       </c>
@@ -3657,12 +3433,11 @@
         <v>72</v>
       </c>
       <c r="E118" s="20"/>
-      <c r="F118" s="23"/>
-      <c r="G118" s="31">
+      <c r="F118" s="26">
         <v>2087.04</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" s="17" t="s">
         <v>100</v>
       </c>
@@ -3678,12 +3453,11 @@
       <c r="E119" s="20">
         <v>101.40864999999999</v>
       </c>
-      <c r="F119" s="23"/>
-      <c r="G119" s="31">
+      <c r="F119" s="26">
         <v>3073.71</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="17" t="s">
         <v>232</v>
       </c>
@@ -3691,12 +3465,9 @@
       <c r="C120" s="15"/>
       <c r="D120" s="19"/>
       <c r="E120" s="20"/>
-      <c r="F120" s="24">
-        <v>0</v>
-      </c>
-      <c r="G120" s="30"/>
-    </row>
-    <row r="121" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F120" s="25"/>
+    </row>
+    <row r="121" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" s="17" t="s">
         <v>233</v>
       </c>
@@ -3704,12 +3475,9 @@
       <c r="C121" s="15"/>
       <c r="D121" s="19"/>
       <c r="E121" s="20"/>
-      <c r="F121" s="24">
-        <v>0.09</v>
-      </c>
-      <c r="G121" s="30"/>
-    </row>
-    <row r="122" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F121" s="25"/>
+    </row>
+    <row r="122" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" s="17" t="s">
         <v>101</v>
       </c>
@@ -3725,12 +3493,11 @@
       <c r="E122" s="20">
         <v>112.11736000000001</v>
       </c>
-      <c r="F122" s="23"/>
-      <c r="G122" s="31">
+      <c r="F122" s="26">
         <v>3064.09</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="17" t="s">
         <v>102</v>
       </c>
@@ -3746,12 +3513,11 @@
       <c r="E123" s="20">
         <v>96.874539999999996</v>
       </c>
-      <c r="F123" s="23"/>
-      <c r="G123" s="31">
+      <c r="F123" s="26">
         <v>2643.69</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="17" t="s">
         <v>103</v>
       </c>
@@ -3767,12 +3533,11 @@
       <c r="E124" s="20">
         <v>77.39067</v>
       </c>
-      <c r="F124" s="23"/>
-      <c r="G124" s="31">
+      <c r="F124" s="26">
         <v>2240.35</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="17" t="s">
         <v>104</v>
       </c>
@@ -3788,12 +3553,11 @@
       <c r="E125" s="20">
         <v>93.944370000000006</v>
       </c>
-      <c r="F125" s="23"/>
-      <c r="G125" s="31">
+      <c r="F125" s="26">
         <v>2962.25</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
         <v>105</v>
       </c>
@@ -3807,14 +3571,11 @@
       <c r="E126" s="20">
         <v>85.563839999999999</v>
       </c>
-      <c r="F126" s="24">
-        <v>0.12</v>
-      </c>
-      <c r="G126" s="31">
+      <c r="F126" s="26">
         <v>3107.09</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="17" t="s">
         <v>106</v>
       </c>
@@ -3830,14 +3591,11 @@
       <c r="E127" s="20">
         <v>70.793009999999995</v>
       </c>
-      <c r="F127" s="24">
-        <v>0.25</v>
-      </c>
-      <c r="G127" s="31">
+      <c r="F127" s="26">
         <v>2476.17</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="17" t="s">
         <v>107</v>
       </c>
@@ -3853,12 +3611,11 @@
       <c r="E128" s="20">
         <v>69.053039999999996</v>
       </c>
-      <c r="F128" s="23"/>
-      <c r="G128" s="31">
+      <c r="F128" s="26">
         <v>2203.79</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="17" t="s">
         <v>108</v>
       </c>
@@ -3872,12 +3629,11 @@
         <v>97</v>
       </c>
       <c r="E129" s="20"/>
-      <c r="F129" s="23"/>
-      <c r="G129" s="31">
+      <c r="F129" s="26">
         <v>3142.93</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="17" t="s">
         <v>234</v>
       </c>
@@ -3887,10 +3643,9 @@
       <c r="E130" s="20">
         <v>102.86976</v>
       </c>
-      <c r="F130" s="23"/>
-      <c r="G130" s="30"/>
-    </row>
-    <row r="131" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F130" s="25"/>
+    </row>
+    <row r="131" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="17" t="s">
         <v>109</v>
       </c>
@@ -3906,12 +3661,11 @@
       <c r="E131" s="20">
         <v>95.671809999999994</v>
       </c>
-      <c r="F131" s="23"/>
-      <c r="G131" s="31">
+      <c r="F131" s="26">
         <v>3436.38</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="17" t="s">
         <v>110</v>
       </c>
@@ -3925,12 +3679,11 @@
         <v>100</v>
       </c>
       <c r="E132" s="20"/>
-      <c r="F132" s="23"/>
-      <c r="G132" s="31">
+      <c r="F132" s="26">
         <v>3681.07</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="17" t="s">
         <v>111</v>
       </c>
@@ -3944,10 +3697,9 @@
       <c r="E133" s="20">
         <v>97.988050000000001</v>
       </c>
-      <c r="F133" s="23"/>
-      <c r="G133" s="30"/>
-    </row>
-    <row r="134" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F133" s="25"/>
+    </row>
+    <row r="134" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="17" t="s">
         <v>112</v>
       </c>
@@ -3963,12 +3715,11 @@
       <c r="E134" s="20">
         <v>92.834220000000002</v>
       </c>
-      <c r="F134" s="23"/>
-      <c r="G134" s="31">
+      <c r="F134" s="26">
         <v>3105.47</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="17" t="s">
         <v>113</v>
       </c>
@@ -3984,14 +3735,11 @@
       <c r="E135" s="20">
         <v>62.562690000000003</v>
       </c>
-      <c r="F135" s="24">
-        <v>1</v>
-      </c>
-      <c r="G135" s="31">
+      <c r="F135" s="26">
         <v>2159.66</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="17" t="s">
         <v>114</v>
       </c>
@@ -4007,14 +3755,11 @@
       <c r="E136" s="20">
         <v>59.301549999999999</v>
       </c>
-      <c r="F136" s="24">
-        <v>7.04</v>
-      </c>
-      <c r="G136" s="31">
+      <c r="F136" s="26">
         <v>2171.62</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="17" t="s">
         <v>115</v>
       </c>
@@ -4028,12 +3773,11 @@
         <v>96</v>
       </c>
       <c r="E137" s="20"/>
-      <c r="F137" s="23"/>
-      <c r="G137" s="31">
+      <c r="F137" s="26">
         <v>2923.14</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="17" t="s">
         <v>116</v>
       </c>
@@ -4047,12 +3791,11 @@
         <v>91</v>
       </c>
       <c r="E138" s="20"/>
-      <c r="F138" s="23"/>
-      <c r="G138" s="31">
+      <c r="F138" s="26">
         <v>2685.39</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="17" t="s">
         <v>117</v>
       </c>
@@ -4068,12 +3811,11 @@
       <c r="E139" s="20">
         <v>48.43094</v>
       </c>
-      <c r="F139" s="23"/>
-      <c r="G139" s="31">
+      <c r="F139" s="26">
         <v>2614.23</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
         <v>118</v>
       </c>
@@ -4089,12 +3831,11 @@
       <c r="E140" s="20">
         <v>95.861930000000001</v>
       </c>
-      <c r="F140" s="23"/>
-      <c r="G140" s="31">
+      <c r="F140" s="26">
         <v>3610.6</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
         <v>119</v>
       </c>
@@ -4110,10 +3851,9 @@
       <c r="E141" s="20">
         <v>116.18217</v>
       </c>
-      <c r="F141" s="23"/>
-      <c r="G141" s="30"/>
-    </row>
-    <row r="142" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F141" s="25"/>
+    </row>
+    <row r="142" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="17" t="s">
         <v>120</v>
       </c>
@@ -4125,10 +3865,9 @@
       </c>
       <c r="D142" s="19"/>
       <c r="E142" s="20"/>
-      <c r="F142" s="23"/>
-      <c r="G142" s="30"/>
-    </row>
-    <row r="143" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F142" s="25"/>
+    </row>
+    <row r="143" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="17" t="s">
         <v>121</v>
       </c>
@@ -4144,14 +3883,11 @@
       <c r="E143" s="20">
         <v>56.698140000000002</v>
       </c>
-      <c r="F143" s="24">
-        <v>12.18</v>
-      </c>
-      <c r="G143" s="31">
+      <c r="F143" s="26">
         <v>2841.06</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="17" t="s">
         <v>122</v>
       </c>
@@ -4167,14 +3903,11 @@
       <c r="E144" s="20">
         <v>93.999420000000001</v>
       </c>
-      <c r="F144" s="24">
-        <v>67.87</v>
-      </c>
-      <c r="G144" s="31">
+      <c r="F144" s="26">
         <v>2965.39</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="17" t="s">
         <v>123</v>
       </c>
@@ -4186,10 +3919,9 @@
       </c>
       <c r="D145" s="19"/>
       <c r="E145" s="20"/>
-      <c r="F145" s="23"/>
-      <c r="G145" s="30"/>
-    </row>
-    <row r="146" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F145" s="25"/>
+    </row>
+    <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="17" t="s">
         <v>124</v>
       </c>
@@ -4205,14 +3937,11 @@
       <c r="E146" s="20">
         <v>103.60254</v>
       </c>
-      <c r="F146" s="24">
-        <v>34.869999999999997</v>
-      </c>
-      <c r="G146" s="31">
+      <c r="F146" s="26">
         <v>3266.31</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="17" t="s">
         <v>125</v>
       </c>
@@ -4226,10 +3955,9 @@
         <v>25</v>
       </c>
       <c r="E147" s="20"/>
-      <c r="F147" s="23"/>
-      <c r="G147" s="30"/>
-    </row>
-    <row r="148" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F147" s="25"/>
+    </row>
+    <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="17" t="s">
         <v>126</v>
       </c>
@@ -4245,12 +3973,11 @@
       <c r="E148" s="20">
         <v>92.913470000000004</v>
       </c>
-      <c r="F148" s="23"/>
-      <c r="G148" s="31">
+      <c r="F148" s="26">
         <v>2771.3</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="17" t="s">
         <v>235</v>
       </c>
@@ -4262,10 +3989,9 @@
         <v>100</v>
       </c>
       <c r="E149" s="20"/>
-      <c r="F149" s="23"/>
-      <c r="G149" s="30"/>
-    </row>
-    <row r="150" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F149" s="25"/>
+    </row>
+    <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="17" t="s">
         <v>127</v>
       </c>
@@ -4281,14 +4007,11 @@
       <c r="E150" s="20">
         <v>108.13563000000001</v>
       </c>
-      <c r="F150" s="24">
-        <v>0.95</v>
-      </c>
-      <c r="G150" s="31">
+      <c r="F150" s="26">
         <v>2285.34</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="17" t="s">
         <v>128</v>
       </c>
@@ -4302,12 +4025,11 @@
         <v>90</v>
       </c>
       <c r="E151" s="20"/>
-      <c r="F151" s="23"/>
-      <c r="G151" s="31">
+      <c r="F151" s="26">
         <v>2447.2199999999998</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="17" t="s">
         <v>236</v>
       </c>
@@ -4315,10 +4037,9 @@
       <c r="C152" s="15"/>
       <c r="D152" s="19"/>
       <c r="E152" s="20"/>
-      <c r="F152" s="23"/>
-      <c r="G152" s="30"/>
-    </row>
-    <row r="153" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F152" s="25"/>
+    </row>
+    <row r="153" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="17" t="s">
         <v>129</v>
       </c>
@@ -4334,14 +4055,11 @@
       <c r="E153" s="20">
         <v>83.630970000000005</v>
       </c>
-      <c r="F153" s="24">
-        <v>0.06</v>
-      </c>
-      <c r="G153" s="31">
+      <c r="F153" s="26">
         <v>3236.03</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="17" t="s">
         <v>130</v>
       </c>
@@ -4357,14 +4075,11 @@
       <c r="E154" s="20">
         <v>45.777650000000001</v>
       </c>
-      <c r="F154" s="24">
-        <v>1.01</v>
-      </c>
-      <c r="G154" s="31">
+      <c r="F154" s="26">
         <v>2066.59</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="17" t="s">
         <v>131</v>
       </c>
@@ -4380,14 +4095,11 @@
       <c r="E155" s="20">
         <v>96.504069999999999</v>
       </c>
-      <c r="F155" s="24">
-        <v>1.33</v>
-      </c>
-      <c r="G155" s="31">
+      <c r="F155" s="26">
         <v>2464.91</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" s="17" t="s">
         <v>132</v>
       </c>
@@ -4403,14 +4115,11 @@
       <c r="E156" s="20">
         <v>81.569929999999999</v>
       </c>
-      <c r="F156" s="24">
-        <v>0.48</v>
-      </c>
-      <c r="G156" s="31">
+      <c r="F156" s="26">
         <v>2382.88</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="17" t="s">
         <v>237</v>
       </c>
@@ -4420,10 +4129,9 @@
       </c>
       <c r="D157" s="19"/>
       <c r="E157" s="20"/>
-      <c r="F157" s="23"/>
-      <c r="G157" s="30"/>
-    </row>
-    <row r="158" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F157" s="25"/>
+    </row>
+    <row r="158" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" s="17" t="s">
         <v>133</v>
       </c>
@@ -4437,12 +4145,11 @@
         <v>27</v>
       </c>
       <c r="E158" s="20"/>
-      <c r="F158" s="23"/>
-      <c r="G158" s="31">
+      <c r="F158" s="26">
         <v>2359.81</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" s="17" t="s">
         <v>134</v>
       </c>
@@ -4456,14 +4163,11 @@
         <v>100</v>
       </c>
       <c r="E159" s="20"/>
-      <c r="F159" s="24">
-        <v>0.92</v>
-      </c>
-      <c r="G159" s="31">
+      <c r="F159" s="26">
         <v>3277.52</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" s="17" t="s">
         <v>135</v>
       </c>
@@ -4473,12 +4177,11 @@
       <c r="C160" s="14"/>
       <c r="D160" s="19"/>
       <c r="E160" s="20"/>
-      <c r="F160" s="23"/>
-      <c r="G160" s="31">
+      <c r="F160" s="26">
         <v>3004.49</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" s="17" t="s">
         <v>136</v>
       </c>
@@ -4490,12 +4193,11 @@
       </c>
       <c r="D161" s="19"/>
       <c r="E161" s="20"/>
-      <c r="F161" s="23"/>
-      <c r="G161" s="31">
+      <c r="F161" s="26">
         <v>2796.7</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" s="17" t="s">
         <v>137</v>
       </c>
@@ -4507,12 +4209,11 @@
       </c>
       <c r="D162" s="19"/>
       <c r="E162" s="20"/>
-      <c r="F162" s="23"/>
-      <c r="G162" s="31">
+      <c r="F162" s="26">
         <v>3159.44</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="17" t="s">
         <v>238</v>
       </c>
@@ -4520,10 +4221,9 @@
       <c r="C163" s="14"/>
       <c r="D163" s="19"/>
       <c r="E163" s="20"/>
-      <c r="F163" s="23"/>
-      <c r="G163" s="30"/>
-    </row>
-    <row r="164" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F163" s="25"/>
+    </row>
+    <row r="164" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A164" s="17" t="s">
         <v>138</v>
       </c>
@@ -4539,12 +4239,11 @@
       <c r="E164" s="20">
         <v>76.25224</v>
       </c>
-      <c r="F164" s="22"/>
-      <c r="G164" s="31">
+      <c r="F164" s="26">
         <v>2403.44</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A165" s="17" t="s">
         <v>139</v>
       </c>
@@ -4560,12 +4259,11 @@
       <c r="E165" s="20">
         <v>39.50291</v>
       </c>
-      <c r="F165" s="22"/>
-      <c r="G165" s="31">
+      <c r="F165" s="26">
         <v>2376.2600000000002</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" s="17" t="s">
         <v>140</v>
       </c>
@@ -4581,12 +4279,11 @@
       <c r="E166" s="20">
         <v>81.096130000000002</v>
       </c>
-      <c r="F166" s="22"/>
-      <c r="G166" s="31">
+      <c r="F166" s="26">
         <v>2740.8</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" s="17" t="s">
         <v>239</v>
       </c>
@@ -4596,10 +4293,9 @@
       </c>
       <c r="D167" s="19"/>
       <c r="E167" s="20"/>
-      <c r="F167" s="22"/>
-      <c r="G167" s="30"/>
-    </row>
-    <row r="168" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F167" s="25"/>
+    </row>
+    <row r="168" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" s="17" t="s">
         <v>240</v>
       </c>
@@ -4607,10 +4303,9 @@
       <c r="C168" s="15"/>
       <c r="D168" s="19"/>
       <c r="E168" s="20"/>
-      <c r="F168" s="22"/>
-      <c r="G168" s="30"/>
-    </row>
-    <row r="169" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F168" s="25"/>
+    </row>
+    <row r="169" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" s="17" t="s">
         <v>241</v>
       </c>
@@ -4618,10 +4313,9 @@
       <c r="C169" s="15"/>
       <c r="D169" s="19"/>
       <c r="E169" s="20"/>
-      <c r="F169" s="22"/>
-      <c r="G169" s="30"/>
-    </row>
-    <row r="170" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F169" s="25"/>
+    </row>
+    <row r="170" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" s="17" t="s">
         <v>141</v>
       </c>
@@ -4633,10 +4327,9 @@
         <v>94</v>
       </c>
       <c r="E170" s="20"/>
-      <c r="F170" s="22"/>
-      <c r="G170" s="30"/>
-    </row>
-    <row r="171" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F170" s="25"/>
+    </row>
+    <row r="171" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" s="17" t="s">
         <v>142</v>
       </c>
@@ -4652,12 +4345,11 @@
       <c r="E171" s="20">
         <v>97.358699999999999</v>
       </c>
-      <c r="F171" s="22"/>
-      <c r="G171" s="31">
+      <c r="F171" s="26">
         <v>3464.18</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A172" s="17" t="s">
         <v>143</v>
       </c>
@@ -4671,10 +4363,9 @@
         <v>96</v>
       </c>
       <c r="E172" s="20"/>
-      <c r="F172" s="22"/>
-      <c r="G172" s="30"/>
-    </row>
-    <row r="173" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F172" s="25"/>
+    </row>
+    <row r="173" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A173" s="17" t="s">
         <v>144</v>
       </c>
@@ -4690,12 +4381,11 @@
       <c r="E173" s="20">
         <v>60.662570000000002</v>
       </c>
-      <c r="F173" s="22"/>
-      <c r="G173" s="31">
+      <c r="F173" s="26">
         <v>2292.7600000000002</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" s="17" t="s">
         <v>242</v>
       </c>
@@ -4707,10 +4397,9 @@
         <v>99</v>
       </c>
       <c r="E174" s="20"/>
-      <c r="F174" s="22"/>
-      <c r="G174" s="30"/>
-    </row>
-    <row r="175" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F174" s="25"/>
+    </row>
+    <row r="175" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" s="17" t="s">
         <v>145</v>
       </c>
@@ -4726,12 +4415,11 @@
       <c r="E175" s="20">
         <v>97.975359999999995</v>
       </c>
-      <c r="F175" s="22"/>
-      <c r="G175" s="31">
+      <c r="F175" s="26">
         <v>2484.04</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" s="17" t="s">
         <v>146</v>
       </c>
@@ -4745,10 +4433,9 @@
         <v>46</v>
       </c>
       <c r="E176" s="20"/>
-      <c r="F176" s="22"/>
-      <c r="G176" s="30"/>
-    </row>
-    <row r="177" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F176" s="25"/>
+    </row>
+    <row r="177" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" s="17" t="s">
         <v>147</v>
       </c>
@@ -4764,12 +4451,11 @@
       <c r="E177" s="20">
         <v>94.681359999999998</v>
       </c>
-      <c r="F177" s="22"/>
-      <c r="G177" s="31">
+      <c r="F177" s="26">
         <v>2634.37</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" s="17" t="s">
         <v>148</v>
       </c>
@@ -4785,12 +4471,11 @@
       <c r="E178" s="20">
         <v>103.48051</v>
       </c>
-      <c r="F178" s="22"/>
-      <c r="G178" s="31">
+      <c r="F178" s="26">
         <v>2457.04</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" s="17" t="s">
         <v>149</v>
       </c>
@@ -4806,12 +4491,11 @@
       <c r="E179" s="20">
         <v>91.746639999999999</v>
       </c>
-      <c r="F179" s="22"/>
-      <c r="G179" s="31">
+      <c r="F179" s="26">
         <v>2564.91</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A180" s="17" t="s">
         <v>243</v>
       </c>
@@ -4819,10 +4503,9 @@
       <c r="C180" s="14"/>
       <c r="D180" s="19"/>
       <c r="E180" s="20"/>
-      <c r="F180" s="22"/>
-      <c r="G180" s="30"/>
-    </row>
-    <row r="181" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F180" s="25"/>
+    </row>
+    <row r="181" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A181" s="17" t="s">
         <v>150</v>
       </c>
@@ -4838,12 +4521,11 @@
       <c r="E181" s="20">
         <v>95.760909999999996</v>
       </c>
-      <c r="F181" s="22"/>
-      <c r="G181" s="31">
+      <c r="F181" s="26">
         <v>3420.74</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" s="17" t="s">
         <v>151</v>
       </c>
@@ -4857,12 +4539,11 @@
         <v>100</v>
       </c>
       <c r="E182" s="20"/>
-      <c r="F182" s="22"/>
-      <c r="G182" s="31">
+      <c r="F182" s="26">
         <v>3583.9</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" s="17" t="s">
         <v>152</v>
       </c>
@@ -4874,10 +4555,9 @@
       </c>
       <c r="D183" s="19"/>
       <c r="E183" s="20"/>
-      <c r="F183" s="22"/>
-      <c r="G183" s="30"/>
-    </row>
-    <row r="184" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F183" s="25"/>
+    </row>
+    <row r="184" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" s="17" t="s">
         <v>153</v>
       </c>
@@ -4893,10 +4573,9 @@
       <c r="E184" s="20">
         <v>101.94494</v>
       </c>
-      <c r="F184" s="22"/>
-      <c r="G184" s="30"/>
-    </row>
-    <row r="185" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F184" s="25"/>
+    </row>
+    <row r="185" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="17" t="s">
         <v>154</v>
       </c>
@@ -4908,10 +4587,9 @@
       </c>
       <c r="D185" s="19"/>
       <c r="E185" s="20"/>
-      <c r="F185" s="22"/>
-      <c r="G185" s="30"/>
-    </row>
-    <row r="186" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F185" s="25"/>
+    </row>
+    <row r="186" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" s="17" t="s">
         <v>155</v>
       </c>
@@ -4927,12 +4605,11 @@
       <c r="E186" s="20">
         <v>115.41941</v>
       </c>
-      <c r="F186" s="22"/>
-      <c r="G186" s="31">
+      <c r="F186" s="26">
         <v>3455.47</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" s="17" t="s">
         <v>156</v>
       </c>
@@ -4948,12 +4625,11 @@
       <c r="E187" s="20">
         <v>92.578789999999998</v>
       </c>
-      <c r="F187" s="22"/>
-      <c r="G187" s="31">
+      <c r="F187" s="26">
         <v>3375.93</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A188" s="17" t="s">
         <v>157</v>
       </c>
@@ -4967,12 +4643,11 @@
         <v>53</v>
       </c>
       <c r="E188" s="20"/>
-      <c r="F188" s="22"/>
-      <c r="G188" s="31">
+      <c r="F188" s="26">
         <v>2085.1</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" s="17" t="s">
         <v>244</v>
       </c>
@@ -4980,10 +4655,9 @@
       <c r="C189" s="14"/>
       <c r="D189" s="19"/>
       <c r="E189" s="20"/>
-      <c r="F189" s="22"/>
-      <c r="G189" s="30"/>
-    </row>
-    <row r="190" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F189" s="25"/>
+    </row>
+    <row r="190" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" s="17" t="s">
         <v>245</v>
       </c>
@@ -4991,10 +4665,9 @@
       <c r="C190" s="15"/>
       <c r="D190" s="19"/>
       <c r="E190" s="20"/>
-      <c r="F190" s="22"/>
-      <c r="G190" s="30"/>
-    </row>
-    <row r="191" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F190" s="25"/>
+    </row>
+    <row r="191" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" s="17" t="s">
         <v>246</v>
       </c>
@@ -5008,12 +4681,11 @@
       <c r="E191" s="20">
         <v>93.212670000000003</v>
       </c>
-      <c r="F191" s="22"/>
-      <c r="G191" s="31">
+      <c r="F191" s="26">
         <v>2512.89</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" s="17" t="s">
         <v>158</v>
       </c>
@@ -5029,12 +4701,11 @@
       <c r="E192" s="20">
         <v>107.30907000000001</v>
       </c>
-      <c r="F192" s="22"/>
-      <c r="G192" s="31">
+      <c r="F192" s="26">
         <v>2737.55</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" s="17" t="s">
         <v>247</v>
       </c>
@@ -5042,10 +4713,9 @@
       <c r="C193" s="15"/>
       <c r="D193" s="19"/>
       <c r="E193" s="20"/>
-      <c r="F193" s="22"/>
-      <c r="G193" s="30"/>
-    </row>
-    <row r="194" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F193" s="25"/>
+    </row>
+    <row r="194" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" s="17" t="s">
         <v>159</v>
       </c>
@@ -5057,12 +4727,11 @@
       </c>
       <c r="D194" s="19"/>
       <c r="E194" s="20"/>
-      <c r="F194" s="22"/>
-      <c r="G194" s="31">
+      <c r="F194" s="26">
         <v>2821.28</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A195" s="17" t="s">
         <v>248</v>
       </c>
@@ -5070,10 +4739,9 @@
       <c r="C195" s="15"/>
       <c r="D195" s="19"/>
       <c r="E195" s="20"/>
-      <c r="F195" s="22"/>
-      <c r="G195" s="30"/>
-    </row>
-    <row r="196" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F195" s="25"/>
+    </row>
+    <row r="196" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="17" t="s">
         <v>160</v>
       </c>
@@ -5089,12 +4757,11 @@
       <c r="E196" s="20">
         <v>108.06798999999999</v>
       </c>
-      <c r="F196" s="22"/>
-      <c r="G196" s="31">
+      <c r="F196" s="26">
         <v>2885.92</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A197" s="17" t="s">
         <v>249</v>
       </c>
@@ -5104,10 +4771,9 @@
       </c>
       <c r="D197" s="19"/>
       <c r="E197" s="20"/>
-      <c r="F197" s="22"/>
-      <c r="G197" s="30"/>
-    </row>
-    <row r="198" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F197" s="25"/>
+    </row>
+    <row r="198" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A198" s="17" t="s">
         <v>161</v>
       </c>
@@ -5123,12 +4789,11 @@
       <c r="E198" s="20">
         <v>71.629429999999999</v>
       </c>
-      <c r="F198" s="22"/>
-      <c r="G198" s="31">
+      <c r="F198" s="26">
         <v>2683.97</v>
       </c>
     </row>
-    <row r="199" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" s="17" t="s">
         <v>162</v>
       </c>
@@ -5142,12 +4807,11 @@
       <c r="E199" s="20">
         <v>93.414429999999996</v>
       </c>
-      <c r="F199" s="22"/>
-      <c r="G199" s="31">
+      <c r="F199" s="26">
         <v>3143.95</v>
       </c>
     </row>
-    <row r="200" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A200" s="17" t="s">
         <v>163</v>
       </c>
@@ -5163,12 +4827,11 @@
       <c r="E200" s="20">
         <v>52.140860000000004</v>
       </c>
-      <c r="F200" s="22"/>
-      <c r="G200" s="31">
+      <c r="F200" s="26">
         <v>2347.71</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A201" s="17" t="s">
         <v>164</v>
       </c>
@@ -5184,12 +4847,11 @@
       <c r="E201" s="20">
         <v>100.51979</v>
       </c>
-      <c r="F201" s="22"/>
-      <c r="G201" s="31">
+      <c r="F201" s="26">
         <v>2710.16</v>
       </c>
     </row>
-    <row r="202" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A202" s="17" t="s">
         <v>250</v>
       </c>
@@ -5197,10 +4859,9 @@
       <c r="C202" s="15"/>
       <c r="D202" s="19"/>
       <c r="E202" s="20"/>
-      <c r="F202" s="22"/>
-      <c r="G202" s="30"/>
-    </row>
-    <row r="203" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F202" s="25"/>
+    </row>
+    <row r="203" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A203" s="17" t="s">
         <v>251</v>
       </c>
@@ -5208,10 +4869,9 @@
       <c r="C203" s="15"/>
       <c r="D203" s="19"/>
       <c r="E203" s="20"/>
-      <c r="F203" s="22"/>
-      <c r="G203" s="30"/>
-    </row>
-    <row r="204" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F203" s="25"/>
+    </row>
+    <row r="204" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A204" s="17" t="s">
         <v>165</v>
       </c>
@@ -5225,12 +4885,11 @@
       <c r="E204" s="20">
         <v>119.65098999999999</v>
       </c>
-      <c r="F204" s="22"/>
-      <c r="G204" s="31">
+      <c r="F204" s="26">
         <v>2462.62</v>
       </c>
     </row>
-    <row r="205" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A205" s="17" t="s">
         <v>166</v>
       </c>
@@ -5244,12 +4903,11 @@
         <v>12</v>
       </c>
       <c r="E205" s="20"/>
-      <c r="F205" s="22"/>
-      <c r="G205" s="31">
+      <c r="F205" s="26">
         <v>2170.2600000000002</v>
       </c>
     </row>
-    <row r="206" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A206" s="17" t="s">
         <v>167</v>
       </c>
@@ -5263,10 +4921,9 @@
         <v>100</v>
       </c>
       <c r="E206" s="20"/>
-      <c r="F206" s="22"/>
-      <c r="G206" s="30"/>
-    </row>
-    <row r="207" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F206" s="25"/>
+    </row>
+    <row r="207" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A207" s="17" t="s">
         <v>168</v>
       </c>
@@ -5282,12 +4939,11 @@
       <c r="E207" s="20">
         <v>92.977940000000004</v>
       </c>
-      <c r="F207" s="22"/>
-      <c r="G207" s="31">
+      <c r="F207" s="26">
         <v>2892.6</v>
       </c>
     </row>
-    <row r="208" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A208" s="17" t="s">
         <v>169</v>
       </c>
@@ -5301,12 +4957,11 @@
         <v>100</v>
       </c>
       <c r="E208" s="20"/>
-      <c r="F208" s="22"/>
-      <c r="G208" s="31">
+      <c r="F208" s="26">
         <v>3223.47</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A209" s="17" t="s">
         <v>170</v>
       </c>
@@ -5318,12 +4973,11 @@
       </c>
       <c r="D209" s="19"/>
       <c r="E209" s="20"/>
-      <c r="F209" s="22"/>
-      <c r="G209" s="31">
+      <c r="F209" s="26">
         <v>2422.27</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A210" s="17" t="s">
         <v>171</v>
       </c>
@@ -5337,10 +4991,9 @@
         <v>23</v>
       </c>
       <c r="E210" s="20"/>
-      <c r="F210" s="22"/>
-      <c r="G210" s="30"/>
-    </row>
-    <row r="211" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F210" s="25"/>
+    </row>
+    <row r="211" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A211" s="17" t="s">
         <v>252</v>
       </c>
@@ -5348,10 +5001,9 @@
       <c r="C211" s="14"/>
       <c r="D211" s="19"/>
       <c r="E211" s="20"/>
-      <c r="F211" s="22"/>
-      <c r="G211" s="30"/>
-    </row>
-    <row r="212" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F211" s="25"/>
+    </row>
+    <row r="212" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A212" s="17" t="s">
         <v>172</v>
       </c>
@@ -5365,12 +5017,11 @@
         <v>77</v>
       </c>
       <c r="E212" s="20"/>
-      <c r="F212" s="22"/>
-      <c r="G212" s="31">
+      <c r="F212" s="26">
         <v>2998.5</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A213" s="17" t="s">
         <v>253</v>
       </c>
@@ -5378,10 +5029,9 @@
       <c r="C213" s="15"/>
       <c r="D213" s="19"/>
       <c r="E213" s="20"/>
-      <c r="F213" s="22"/>
-      <c r="G213" s="30"/>
-    </row>
-    <row r="214" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F213" s="25"/>
+    </row>
+    <row r="214" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A214" s="17" t="s">
         <v>173</v>
       </c>
@@ -5397,12 +5047,11 @@
       <c r="E214" s="20">
         <v>98.71</v>
       </c>
-      <c r="F214" s="22"/>
-      <c r="G214" s="31">
+      <c r="F214" s="26">
         <v>3271.77</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A215" s="17" t="s">
         <v>174</v>
       </c>
@@ -5418,12 +5067,11 @@
       <c r="E215" s="20">
         <v>101.61394</v>
       </c>
-      <c r="F215" s="22"/>
-      <c r="G215" s="31">
+      <c r="F215" s="26">
         <v>2360.61</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A216" s="17" t="s">
         <v>175</v>
       </c>
@@ -5437,12 +5085,11 @@
         <v>26</v>
       </c>
       <c r="E216" s="20"/>
-      <c r="F216" s="22"/>
-      <c r="G216" s="31">
+      <c r="F216" s="26">
         <v>2282.06</v>
       </c>
     </row>
-    <row r="217" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A217" s="17" t="s">
         <v>176</v>
       </c>
@@ -5458,12 +5105,11 @@
       <c r="E217" s="20">
         <v>76.421729999999997</v>
       </c>
-      <c r="F217" s="22"/>
-      <c r="G217" s="31">
+      <c r="F217" s="26">
         <v>2492.4499999999998</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A218" s="17" t="s">
         <v>254</v>
       </c>
@@ -5471,10 +5117,9 @@
       <c r="C218" s="14"/>
       <c r="D218" s="19"/>
       <c r="E218" s="20"/>
-      <c r="F218" s="22"/>
-      <c r="G218" s="30"/>
-    </row>
-    <row r="219" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F218" s="25"/>
+    </row>
+    <row r="219" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A219" s="17" t="s">
         <v>177</v>
       </c>
@@ -5490,12 +5135,11 @@
       <c r="E219" s="20">
         <v>73.258809999999997</v>
       </c>
-      <c r="F219" s="22"/>
-      <c r="G219" s="31">
+      <c r="F219" s="26">
         <v>2292.25</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A220" s="17" t="s">
         <v>178</v>
       </c>
@@ -5511,12 +5155,11 @@
       <c r="E220" s="20">
         <v>95.672520000000006</v>
       </c>
-      <c r="F220" s="22"/>
-      <c r="G220" s="31">
+      <c r="F220" s="26">
         <v>3110.22</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A221" s="17" t="s">
         <v>179</v>
       </c>
@@ -5532,12 +5175,11 @@
       <c r="E221" s="20">
         <v>92.629850000000005</v>
       </c>
-      <c r="F221" s="22"/>
-      <c r="G221" s="31">
+      <c r="F221" s="26">
         <v>3465.33</v>
       </c>
     </row>
-    <row r="222" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A222" s="17" t="s">
         <v>180</v>
       </c>
@@ -5553,12 +5195,11 @@
       <c r="E222" s="20">
         <v>103.55911999999999</v>
       </c>
-      <c r="F222" s="22"/>
-      <c r="G222" s="31">
+      <c r="F222" s="26">
         <v>3034.26</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A223" s="17" t="s">
         <v>181</v>
       </c>
@@ -5568,10 +5209,9 @@
       <c r="C223" s="14"/>
       <c r="D223" s="19"/>
       <c r="E223" s="20"/>
-      <c r="F223" s="22"/>
-      <c r="G223" s="30"/>
-    </row>
-    <row r="224" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F223" s="25"/>
+    </row>
+    <row r="224" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A224" s="17" t="s">
         <v>182</v>
       </c>
@@ -5587,12 +5227,11 @@
       <c r="E224" s="20">
         <v>94.91525</v>
       </c>
-      <c r="F224" s="21"/>
-      <c r="G224" s="31">
+      <c r="F224" s="26">
         <v>2117.52</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A225" s="17" t="s">
         <v>183</v>
       </c>
@@ -5608,12 +5247,11 @@
       <c r="E225" s="20">
         <v>83.243039999999993</v>
       </c>
-      <c r="F225" s="21"/>
-      <c r="G225" s="31">
+      <c r="F225" s="26">
         <v>2032.39</v>
       </c>
     </row>
-    <row r="226" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A226" s="17" t="s">
         <v>184</v>
       </c>
@@ -5627,12 +5265,11 @@
         <v>96</v>
       </c>
       <c r="E226" s="20"/>
-      <c r="F226" s="21"/>
-      <c r="G226" s="31">
+      <c r="F226" s="26">
         <v>2538.62</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A227" s="17" t="s">
         <v>185</v>
       </c>
@@ -5646,12 +5283,11 @@
         <v>43</v>
       </c>
       <c r="E227" s="20"/>
-      <c r="F227" s="21"/>
-      <c r="G227" s="31">
+      <c r="F227" s="26">
         <v>2065.67</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A228" s="17" t="s">
         <v>186</v>
       </c>
@@ -5665,12 +5301,11 @@
         <v>13</v>
       </c>
       <c r="E228" s="20"/>
-      <c r="F228"/>
-      <c r="G228" s="31">
+      <c r="F228" s="26">
         <v>2161.06</v>
       </c>
     </row>
-    <row r="229" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A229" s="17" t="s">
         <v>255</v>
       </c>
@@ -5678,10 +5313,9 @@
       <c r="C229" s="14"/>
       <c r="D229" s="19"/>
       <c r="E229" s="20"/>
-      <c r="F229"/>
-      <c r="G229" s="30"/>
-    </row>
-    <row r="230" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F229" s="25"/>
+    </row>
+    <row r="230" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A230" s="17" t="s">
         <v>187</v>
       </c>
@@ -5695,10 +5329,9 @@
         <v>96</v>
       </c>
       <c r="E230" s="20"/>
-      <c r="F230"/>
-      <c r="G230" s="30"/>
-    </row>
-    <row r="231" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F230" s="25"/>
+    </row>
+    <row r="231" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A231" s="17" t="s">
         <v>256</v>
       </c>
@@ -5706,10 +5339,9 @@
       <c r="C231" s="15"/>
       <c r="D231" s="19"/>
       <c r="E231" s="20"/>
-      <c r="F231"/>
-      <c r="G231" s="30"/>
-    </row>
-    <row r="232" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F231" s="25"/>
+    </row>
+    <row r="232" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A232" s="17" t="s">
         <v>188</v>
       </c>
@@ -5725,12 +5357,11 @@
       <c r="E232" s="20">
         <v>93.097970000000004</v>
       </c>
-      <c r="F232"/>
-      <c r="G232" s="31">
+      <c r="F232" s="26">
         <v>2725.15</v>
       </c>
     </row>
-    <row r="233" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A233" s="17" t="s">
         <v>189</v>
       </c>
@@ -5746,12 +5377,11 @@
       <c r="E233" s="20">
         <v>103.0664</v>
       </c>
-      <c r="F233"/>
-      <c r="G233" s="31">
+      <c r="F233" s="26">
         <v>3326.45</v>
       </c>
     </row>
-    <row r="234" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A234" s="17" t="s">
         <v>190</v>
       </c>
@@ -5767,12 +5397,11 @@
       <c r="E234" s="20">
         <v>95.891220000000004</v>
       </c>
-      <c r="F234"/>
-      <c r="G234" s="31">
+      <c r="F234" s="26">
         <v>3516.73</v>
       </c>
     </row>
-    <row r="235" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A235" s="17" t="s">
         <v>191</v>
       </c>
@@ -5786,12 +5415,11 @@
         <v>98</v>
       </c>
       <c r="E235" s="20"/>
-      <c r="F235"/>
-      <c r="G235" s="31">
+      <c r="F235" s="26">
         <v>2731.4</v>
       </c>
     </row>
-    <row r="236" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A236" s="17" t="s">
         <v>257</v>
       </c>
@@ -5799,10 +5427,9 @@
       <c r="C236" s="14"/>
       <c r="D236" s="19"/>
       <c r="E236" s="20"/>
-      <c r="F236"/>
-      <c r="G236" s="30"/>
-    </row>
-    <row r="237" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F236" s="25"/>
+    </row>
+    <row r="237" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A237" s="17" t="s">
         <v>258</v>
       </c>
@@ -5814,10 +5441,9 @@
         <v>83</v>
       </c>
       <c r="E237" s="20"/>
-      <c r="F237"/>
-      <c r="G237" s="30"/>
-    </row>
-    <row r="238" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F237" s="25"/>
+    </row>
+    <row r="238" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A238" s="17" t="s">
         <v>192</v>
       </c>
@@ -5833,12 +5459,11 @@
       <c r="E238" s="20">
         <v>53.564329999999998</v>
       </c>
-      <c r="F238"/>
-      <c r="G238" s="31">
+      <c r="F238" s="26">
         <v>2211.3000000000002</v>
       </c>
     </row>
-    <row r="239" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A239" s="17" t="s">
         <v>193</v>
       </c>
@@ -5854,12 +5479,11 @@
       <c r="E239" s="20">
         <v>102.05482000000001</v>
       </c>
-      <c r="F239"/>
-      <c r="G239" s="31">
+      <c r="F239" s="26">
         <v>3223.72</v>
       </c>
     </row>
-    <row r="240" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A240" s="17" t="s">
         <v>194</v>
       </c>
@@ -5873,12 +5497,11 @@
         <v>97</v>
       </c>
       <c r="E240" s="20"/>
-      <c r="F240"/>
-      <c r="G240" s="31">
+      <c r="F240" s="26">
         <v>3171.2</v>
       </c>
     </row>
-    <row r="241" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A241" s="17" t="s">
         <v>195</v>
       </c>
@@ -5892,12 +5515,11 @@
         <v>100</v>
       </c>
       <c r="E241" s="20"/>
-      <c r="F241"/>
-      <c r="G241" s="31">
+      <c r="F241" s="26">
         <v>3458.41</v>
       </c>
     </row>
-    <row r="242" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A242" s="17" t="s">
         <v>196</v>
       </c>
@@ -5913,12 +5535,11 @@
       <c r="E242" s="20">
         <v>100.19121</v>
       </c>
-      <c r="F242"/>
-      <c r="G242" s="31">
+      <c r="F242" s="26">
         <v>3748.36</v>
       </c>
     </row>
-    <row r="243" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A243" s="17" t="s">
         <v>197</v>
       </c>
@@ -5934,12 +5555,11 @@
       <c r="E243" s="20">
         <v>104.27171</v>
       </c>
-      <c r="F243"/>
-      <c r="G243" s="31">
+      <c r="F243" s="26">
         <v>2829.47</v>
       </c>
     </row>
-    <row r="244" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A244" s="17" t="s">
         <v>259</v>
       </c>
@@ -5947,10 +5567,9 @@
       <c r="C244" s="14"/>
       <c r="D244" s="19"/>
       <c r="E244" s="20"/>
-      <c r="F244"/>
-      <c r="G244" s="30"/>
-    </row>
-    <row r="245" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F244" s="25"/>
+    </row>
+    <row r="245" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A245" s="17" t="s">
         <v>198</v>
       </c>
@@ -5966,12 +5585,11 @@
       <c r="E245" s="20">
         <v>97.424149999999997</v>
       </c>
-      <c r="F245"/>
-      <c r="G245" s="31">
+      <c r="F245" s="26">
         <v>2581.11</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A246" s="17" t="s">
         <v>260</v>
       </c>
@@ -5979,10 +5597,9 @@
       <c r="C246" s="15"/>
       <c r="D246" s="19"/>
       <c r="E246" s="20"/>
-      <c r="F246"/>
-      <c r="G246" s="30"/>
-    </row>
-    <row r="247" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F246" s="25"/>
+    </row>
+    <row r="247" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A247" s="17" t="s">
         <v>199</v>
       </c>
@@ -5998,12 +5615,11 @@
       <c r="E247" s="20">
         <v>81.740899999999996</v>
       </c>
-      <c r="F247"/>
-      <c r="G247" s="31">
+      <c r="F247" s="26">
         <v>2740.23</v>
       </c>
     </row>
-    <row r="248" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A248" s="17" t="s">
         <v>200</v>
       </c>
@@ -6019,12 +5635,11 @@
       <c r="E248" s="20">
         <v>97.750380000000007</v>
       </c>
-      <c r="F248"/>
-      <c r="G248" s="31">
+      <c r="F248" s="26">
         <v>2631.9</v>
       </c>
     </row>
-    <row r="249" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A249" s="17" t="s">
         <v>201</v>
       </c>
@@ -6040,12 +5655,11 @@
       <c r="E249" s="20">
         <v>86.718249999999998</v>
       </c>
-      <c r="F249"/>
-      <c r="G249" s="31">
+      <c r="F249" s="26">
         <v>2019.71</v>
       </c>
     </row>
-    <row r="250" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A250" s="17" t="s">
         <v>261</v>
       </c>
@@ -6053,10 +5667,9 @@
       <c r="C250" s="14"/>
       <c r="D250" s="19"/>
       <c r="E250" s="20"/>
-      <c r="F250"/>
-      <c r="G250" s="30"/>
-    </row>
-    <row r="251" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F250" s="25"/>
+    </row>
+    <row r="251" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A251" s="17" t="s">
         <v>202</v>
       </c>
@@ -6068,10 +5681,9 @@
       </c>
       <c r="D251" s="19"/>
       <c r="E251" s="20"/>
-      <c r="F251"/>
-      <c r="G251" s="30"/>
-    </row>
-    <row r="252" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F251" s="25"/>
+    </row>
+    <row r="252" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A252" s="17" t="s">
         <v>203</v>
       </c>
@@ -6085,12 +5697,11 @@
         <v>69</v>
       </c>
       <c r="E252" s="20"/>
-      <c r="F252"/>
-      <c r="G252" s="31">
+      <c r="F252" s="26">
         <v>2816.25</v>
       </c>
     </row>
-    <row r="253" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A253" s="17" t="s">
         <v>204</v>
       </c>
@@ -6102,10 +5713,9 @@
       </c>
       <c r="D253" s="19"/>
       <c r="E253" s="20"/>
-      <c r="F253"/>
-      <c r="G253" s="30"/>
-    </row>
-    <row r="254" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F253" s="25"/>
+    </row>
+    <row r="254" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A254" s="17" t="s">
         <v>262</v>
       </c>
@@ -6113,10 +5723,9 @@
       <c r="C254" s="14"/>
       <c r="D254" s="19"/>
       <c r="E254" s="20"/>
-      <c r="F254"/>
-      <c r="G254" s="30"/>
-    </row>
-    <row r="255" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F254" s="25"/>
+    </row>
+    <row r="255" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A255" s="17" t="s">
         <v>263</v>
       </c>
@@ -6124,10 +5733,9 @@
       <c r="C255" s="15"/>
       <c r="D255" s="19"/>
       <c r="E255" s="20"/>
-      <c r="F255"/>
-      <c r="G255" s="30"/>
-    </row>
-    <row r="256" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F255" s="25"/>
+    </row>
+    <row r="256" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A256" s="17" t="s">
         <v>205</v>
       </c>
@@ -6141,11 +5749,11 @@
         <v>49</v>
       </c>
       <c r="E256" s="20"/>
-      <c r="G256" s="31">
+      <c r="F256" s="26">
         <v>2067.5700000000002</v>
       </c>
     </row>
-    <row r="257" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A257" s="17" t="s">
         <v>264</v>
       </c>
@@ -6153,9 +5761,9 @@
       <c r="C257" s="15"/>
       <c r="D257" s="19"/>
       <c r="E257" s="20"/>
-      <c r="G257" s="30"/>
-    </row>
-    <row r="258" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F257" s="25"/>
+    </row>
+    <row r="258" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A258" s="17" t="s">
         <v>206</v>
       </c>
@@ -6171,11 +5779,11 @@
       <c r="E258" s="20">
         <v>92.669409999999999</v>
       </c>
-      <c r="G258" s="31">
+      <c r="F258" s="26">
         <v>1873.04</v>
       </c>
     </row>
-    <row r="259" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A259" s="17" t="s">
         <v>207</v>
       </c>
@@ -6188,53 +5796,53 @@
       <c r="D259" s="19">
         <v>40</v>
       </c>
-      <c r="G259" s="31">
+      <c r="F259" s="26">
         <v>2237.75</v>
       </c>
     </row>
-    <row r="260" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A260" s="17"/>
       <c r="B260" s="18"/>
       <c r="C260" s="14"/>
-      <c r="G260" s="30"/>
-    </row>
-    <row r="261" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="F260" s="25"/>
+    </row>
+    <row r="261" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A261" s="17"/>
       <c r="B261" s="18"/>
       <c r="C261" s="14"/>
     </row>
-    <row r="262" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A262" s="14"/>
       <c r="C262" s="15"/>
     </row>
-    <row r="263" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A263" s="15"/>
     </row>
-    <row r="264" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A264" s="15"/>
     </row>
-    <row r="265" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A265" s="15"/>
     </row>
-    <row r="266" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A266" s="15"/>
     </row>
-    <row r="267" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A267" s="15"/>
     </row>
-    <row r="268" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A268" s="15"/>
     </row>
-    <row r="269" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A269" s="15"/>
     </row>
-    <row r="270" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A270" s="15"/>
     </row>
-    <row r="271" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A271" s="15"/>
     </row>
-    <row r="272" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A272" s="15"/>
     </row>
     <row r="273" spans="1:1" ht="15" x14ac:dyDescent="0.25">

</xml_diff>